<commit_message>
Update sample sheet inscription type field value (#40)
* updating gitignore

* udpating inscription type column

* updating sample run command on readme

* updating readme

* fixing file
</commit_message>
<xml_diff>
--- a/sample/legacy_spreadsheet_sample.xlsx
+++ b/sample/legacy_spreadsheet_sample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Empresa" sheetId="1" state="visible" r:id="rId2"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
   <si>
     <t xml:space="preserve">* Nome da Empresa</t>
   </si>
@@ -78,7 +78,7 @@
     <t xml:space="preserve"> Vinta Servicos e Solucoes Tec</t>
   </si>
   <si>
-    <t xml:space="preserve">9</t>
+    <t xml:space="preserve">2</t>
   </si>
   <si>
     <t xml:space="preserve">99999999000999</t>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9</t>
   </si>
   <si>
     <t xml:space="preserve">999999</t>
@@ -574,13 +577,13 @@
   </sheetPr>
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="R2" activeCellId="0" sqref="R2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.71"/>
@@ -681,43 +684,43 @@
         <v>22</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="H2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="J2" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="K2" s="7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -732,13 +735,13 @@
   </sheetPr>
   <dimension ref="A1:AD1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="32.57"/>
@@ -746,39 +749,39 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="36.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="34.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="37.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="15.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="23.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>6</v>
@@ -790,19 +793,19 @@
         <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="P1" s="3" t="s">
         <v>13</v>
@@ -830,61 +833,61 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L2" s="7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O2" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P2" s="7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S2" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -21848,7 +21851,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -21869,7 +21872,7 @@
       <selection pane="bottomLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.4609375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="34.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="35.29"/>
@@ -21878,7 +21881,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="20.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="29.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="21.14"/>
@@ -21888,192 +21891,192 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="26.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="25.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="23.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="27.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="23.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="27.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="31.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="28" style="0" width="35.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Q1" s="12" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="R1" s="12" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="S1" s="12" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="T1" s="12" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U1" s="12" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="V1" s="12" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="W1" s="12" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="X1" s="12" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="Y1" s="12" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="Z1" s="12" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="AA1" s="12" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="AB1" s="12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="AC1" s="12" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="AD1" s="12" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B2" s="5"/>
       <c r="C2" s="5" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>22</v>
       </c>
       <c r="Q2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="Y2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="Z2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AB2" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="S2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="U2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB2" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC2" s="13" t="s">
-        <v>48</v>
-      </c>
       <c r="AD2" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -54014,14 +54017,14 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A3:A1000" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="A3:A1000" type="list">
       <formula1>Funcionários!$A$2:$A$1000</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>